<commit_message>
update nội dung được chỉnh sửa
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Quet Barcode thu quy/AF0324_Xac nhan thu quy.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Quet Barcode thu quy/AF0324_Xac nhan thu quy.xlsx
@@ -2184,18 +2184,6 @@
     <t>@SQL0004</t>
   </si>
   <si>
-    <t>@OrderStatus
-@DivisionID
-@OrderID
-@DeliveryStatus</t>
-  </si>
-  <si>
-    <t>3
-@@DivisionID
-@@OrderID
-1</t>
-  </si>
-  <si>
     <t>Sau khi thực thi @SQL0002 tiến hành thực thi câu @SQL0004 để Update tình trạng đơn hàng nếu các phiếu điều phối đã hoàn tất</t>
   </si>
   <si>
@@ -2220,11 +2208,23 @@
 AND SOrderID = @SOrderID AND
 (SELECT SUM(ActualQuantity) FROM AT2007 AT07
 INNER JOIN AT2006 AT06 ON AT06.DivisionID= AT07.DivisionID AND AT06.VoucherID=AT07.VoucherID
-WHERE AT07.DivisioniD = @DivisionID AND AT06.OrderID = @OrderID AND AT06.DeliveryStatus = 1)
+WHERE AT07.DivisionID = @DivisionID AND AT06.OrderID = @OrderID AND AT06.DeliveryStatus = 1)
  = 
 (SELECT OrderQuantity FROM OT2002 OT02
 INNER JOIN AT2006 AT06 ON AT06.DivisionID = OT02.DivisionID AND AT06.OrderID=OT02.SOrderID
 WHERE OT02.DivisionID=@DivisionID AND AT06.OrderID=@OrderID)</t>
+  </si>
+  <si>
+    <t>@OrderStatus
+@DivisionID
+@SOrderID=@OrderID
+@DeliveryStatus</t>
+  </si>
+  <si>
+    <t>3
+@@DivisionID
+@@SOrderID
+1</t>
   </si>
 </sst>
 </file>
@@ -6566,7 +6566,7 @@
         <v>170</v>
       </c>
       <c r="E6" s="206" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F6" s="207"/>
       <c r="G6" s="207"/>
@@ -11352,7 +11352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1048467"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D6" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="K8" sqref="K8:N8"/>
     </sheetView>
   </sheetViews>
@@ -11372,7 +11372,7 @@
     <col min="12" max="12" width="11.28515625" style="22" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" style="23" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" style="23" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" style="23" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="23" customWidth="1"/>
     <col min="16" max="18" width="14.140625" style="23" customWidth="1"/>
     <col min="19" max="19" width="36.7109375" style="23" customWidth="1"/>
     <col min="20" max="21" width="12.7109375" style="23" customWidth="1"/>
@@ -11682,7 +11682,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="163" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E8" s="164" t="s">
         <v>214</v>
@@ -11701,16 +11701,16 @@
         <v>217</v>
       </c>
       <c r="K8" s="250" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L8" s="251"/>
       <c r="M8" s="251"/>
       <c r="N8" s="252"/>
       <c r="O8" s="164" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P8" s="164" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="Q8" s="165" t="s">
         <v>167</v>
@@ -11719,7 +11719,7 @@
         <v>184</v>
       </c>
       <c r="S8" s="167" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="34" customFormat="1" ht="11.25">
@@ -14241,7 +14241,7 @@
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="C15" s="117" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
@@ -14366,7 +14366,7 @@
     </row>
     <row r="26" spans="1:10" ht="208.5" customHeight="1">
       <c r="A26" s="262" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B26" s="263"/>
       <c r="C26" s="263"/>

</xml_diff>